<commit_message>
Major revision to CAN ID Protocol
</commit_message>
<xml_diff>
--- a/Renegade-BLT CAN Protocol and Link Budgets.xlsx
+++ b/Renegade-BLT CAN Protocol and Link Budgets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Morgan\Documents\Rockets\BLT\Akheilos\Avionics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4507DD11-9D76-4B40-8A9D-19E7C5BDE334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88E24127-353F-4441-A217-66D064A91E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{43E521ED-7EE3-47F0-8CB3-A655151C58BF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{43E521ED-7EE3-47F0-8CB3-A655151C58BF}"/>
   </bookViews>
   <sheets>
     <sheet name="CAN" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="213">
   <si>
     <t>Sensor</t>
   </si>
@@ -176,21 +176,6 @@
     <t>Reciever Node ID Bits</t>
   </si>
   <si>
-    <t>State Bit number to set (of 64 possible bits per node) A</t>
-  </si>
-  <si>
-    <t>State Bit number to set (of 64 possible bits per node) B</t>
-  </si>
-  <si>
-    <t>State Bit B</t>
-  </si>
-  <si>
-    <t>State Bit A</t>
-  </si>
-  <si>
-    <t>Bonus bit???</t>
-  </si>
-  <si>
     <t>In this design, 3 types of message</t>
   </si>
   <si>
@@ -203,9 +188,6 @@
     <t>State Report Frame</t>
   </si>
   <si>
-    <t>Byte new sample bits in ID A are all 0, but no ext ID means all data bits are the state report</t>
-  </si>
-  <si>
     <t>Need to leave some overhead for requesting resend of error frames?</t>
   </si>
   <si>
@@ -632,9 +614,6 @@
     <t>Pin</t>
   </si>
   <si>
-    <t>Prioity bit - lower number wins, so 0 for command and state report frames, 1 for data frames</t>
-  </si>
-  <si>
     <t>Priority Bit - 0</t>
   </si>
   <si>
@@ -644,15 +623,6 @@
     <t>Central control node (in LCC) is always node 000 so it always has higher message priority</t>
   </si>
   <si>
-    <t>Command and State Report frames only travel one direction on the bus (central to remote nodes for command, inverse for state report) - don't need other identifier information to determine these frame types</t>
-  </si>
-  <si>
-    <t>*There are 7 free bits in Command Frame ID that could fit a whole command. I think I want to keep the current setup with two commands in the extended ID and all zeroes in the command standard ID, but there is potential for expanded use here.</t>
-  </si>
-  <si>
-    <t>Each actuation command can pack two commands per frame in - to be used only for synced orders like opening two valves in a simultaneous command</t>
-  </si>
-  <si>
     <t>Need a field in code to declare which CAN bus this is on so the node IDs (other than 000) can be duplicated</t>
   </si>
   <si>
@@ -663,6 +633,51 @@
   </si>
   <si>
     <t>SV DB 37</t>
+  </si>
+  <si>
+    <t>DATA Bytes (0-8)</t>
+  </si>
+  <si>
+    <t>Zeros</t>
+  </si>
+  <si>
+    <t>State Bit Address</t>
+  </si>
+  <si>
+    <t>State Bit Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Frame </t>
+  </si>
+  <si>
+    <t>Custom packing</t>
+  </si>
+  <si>
+    <t>State Report Frames</t>
+  </si>
+  <si>
+    <t>Full 8 byte package correlating to state lookup table</t>
+  </si>
+  <si>
+    <t>UNUSED</t>
+  </si>
+  <si>
+    <t>Custom packing fills bytes up to 5 samples or next sample overflows, zeros for empty bits</t>
+  </si>
+  <si>
+    <t>State table fills all 64 bits of the Data Bytes</t>
+  </si>
+  <si>
+    <t>Repeat for 1 commanded action per Data Byte (up to 8 commands per frame)</t>
+  </si>
+  <si>
+    <t>From node other than 000, priority bit 1</t>
+  </si>
+  <si>
+    <t>From node in range 001-111, priority bit 0</t>
+  </si>
+  <si>
+    <t>From node 000, address to a node in range 001-111, priority bit 0</t>
   </si>
 </sst>
 </file>
@@ -727,7 +742,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -785,30 +800,6 @@
         <color indexed="64"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -892,6 +883,15 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -932,12 +932,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
@@ -945,26 +974,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection hidden="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -977,13 +1000,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
@@ -992,34 +1015,60 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1338,7 +1387,7 @@
   <dimension ref="A2:P38"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1368,7 +1417,7 @@
         <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1384,7 +1433,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="C4">
         <v>500000</v>
@@ -1395,7 +1444,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="C5">
         <v>500000</v>
@@ -1403,10 +1452,10 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -1414,10 +1463,10 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -1431,11 +1480,11 @@
       <c r="C10" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="11">
+      <c r="D10" s="9">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>3</v>
@@ -1467,203 +1516,203 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="42">
+      <c r="C13" s="37">
         <v>1</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="42">
+      <c r="F13" s="37">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="44">
+      <c r="C14" s="39">
         <v>11</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="39">
         <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="C15" s="44">
+      <c r="C15" s="39">
         <v>1</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="44">
+      <c r="C16" s="39">
         <v>1</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="43" t="s">
+      <c r="B17" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="44">
+      <c r="C17" s="39">
         <v>1</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="F17" s="44">
+      <c r="F17" s="39">
         <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="43" t="s">
+      <c r="B18" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="44">
+      <c r="C18" s="39">
         <v>4</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="F18" s="44">
+      <c r="F18" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="43" t="s">
+      <c r="B19" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="47">
+      <c r="C19" s="42">
         <f>D10*8</f>
         <v>64</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="F19" s="44">
+      <c r="F19" s="39">
         <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="43" t="s">
+      <c r="B20" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="C20" s="44">
+      <c r="C20" s="39">
         <v>15</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="39">
         <v>4</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="C21" s="44">
+      <c r="C21" s="39">
         <v>1</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="38" t="s">
         <v>18</v>
       </c>
-      <c r="F21" s="47">
+      <c r="F21" s="42">
         <f>D10*8</f>
         <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="43" t="s">
+      <c r="B22" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="44">
+      <c r="C22" s="39">
         <v>1</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="F22" s="44">
+      <c r="F22" s="39">
         <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="C23" s="44">
+      <c r="C23" s="39">
         <v>1</v>
       </c>
-      <c r="E23" s="43" t="s">
+      <c r="E23" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="44">
+      <c r="F23" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="44">
+      <c r="C24" s="39">
         <v>7</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F24" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="45" t="s">
+      <c r="B25" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="C25" s="46">
+      <c r="C25" s="41">
         <f>MROUND(((((34+(8*D10))-1)/4)), 1)</f>
         <v>24</v>
       </c>
-      <c r="E25" s="43" t="s">
+      <c r="E25" s="38" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="44">
+      <c r="F25" s="39">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="44">
+      <c r="F26" s="39">
         <v>7</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="45" t="s">
+      <c r="E27" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="F27" s="46">
+      <c r="F27" s="41">
         <f>MROUND(((((54+(8*D10))-1)/4)), 1)</f>
         <v>29</v>
       </c>
@@ -1691,29 +1740,41 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B30" s="22"/>
-      <c r="C30" s="22"/>
+      <c r="B30" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D31" s="23" t="s">
-        <v>206</v>
-      </c>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16" t="s">
-        <v>120</v>
-      </c>
-      <c r="J31" s="16"/>
-      <c r="K31" s="16"/>
+      <c r="C31" t="s">
+        <v>73</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" t="s">
+        <v>75</v>
+      </c>
+      <c r="F31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="13"/>
+      <c r="H31" s="13"/>
+      <c r="I31" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J31" s="13"/>
+      <c r="K31" s="13"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1736,10 +1797,10 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="B36" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C36">
         <f>SUM('Sensor Table'!F:F)</f>
@@ -1747,8 +1808,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B37" s="21" t="s">
-        <v>112</v>
+      <c r="B37" s="18" t="s">
+        <v>106</v>
       </c>
       <c r="C37">
         <f>C36/4</f>
@@ -1758,7 +1819,7 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C38">
         <f>C37*F28</f>
@@ -1767,9 +1828,8 @@
       <c r="D38" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="D31:F31"/>
+  <mergeCells count="1">
+    <mergeCell ref="B30:F30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1780,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E249A31-2D1C-4402-A87A-846C4C4029BB}">
   <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,25 +1852,31 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>46</v>
+      </c>
+      <c r="B2" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>211</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1827,98 +1893,111 @@
       </c>
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="7">
+      <c r="B8" s="32">
         <v>0</v>
       </c>
-      <c r="C8" s="12">
+      <c r="C8" s="10">
         <v>1</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="10">
         <v>2</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="10">
         <v>3</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="10">
         <v>4</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="10">
         <v>5</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="10">
         <v>6</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="10">
         <v>7</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="10">
         <v>8</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="10">
         <v>9</v>
       </c>
-      <c r="L8" s="13">
+      <c r="L8" s="11">
         <v>10</v>
       </c>
-      <c r="M8" s="10"/>
+      <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>192</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="21"/>
+      <c r="M9" s="7"/>
+    </row>
+    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D10" s="28"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="29"/>
+      <c r="J10" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="K10" s="28"/>
+      <c r="L10" s="29"/>
+    </row>
+    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" s="50" t="s">
+        <v>191</v>
+      </c>
+      <c r="C11" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="32"/>
-      <c r="E9" s="33"/>
-      <c r="F9" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
-      <c r="I9" s="34"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="L9" s="25"/>
-      <c r="M9" s="9"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10" s="36" t="s">
-        <v>198</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="32"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="15"/>
-    </row>
-    <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="36" t="s">
-        <v>198</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>41</v>
-      </c>
-      <c r="D11" s="32"/>
-      <c r="E11" s="33"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="33" t="s">
+        <v>199</v>
+      </c>
+      <c r="G11" s="34"/>
+      <c r="H11" s="34"/>
+      <c r="I11" s="34"/>
+      <c r="J11" s="34"/>
+      <c r="K11" s="34"/>
+      <c r="L11" s="35"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -1934,173 +2013,253 @@
       </c>
     </row>
     <row r="20" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="37">
+      <c r="B20" s="32">
         <v>0</v>
       </c>
-      <c r="C20" s="12">
+      <c r="C20" s="10">
         <v>1</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="10">
         <v>2</v>
       </c>
-      <c r="E20" s="8">
+      <c r="E20" s="10">
         <v>3</v>
       </c>
-      <c r="F20" s="8">
+      <c r="F20" s="10">
         <v>4</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="10">
         <v>5</v>
       </c>
-      <c r="H20" s="8">
+      <c r="H20" s="10">
         <v>6</v>
       </c>
-      <c r="I20" s="8">
+      <c r="I20" s="10">
         <v>7</v>
       </c>
-      <c r="J20" s="8">
+      <c r="J20" s="10">
         <v>8</v>
       </c>
-      <c r="K20" s="8">
+      <c r="K20" s="10">
         <v>9</v>
       </c>
-      <c r="L20" s="12">
+      <c r="L20" s="10">
         <v>10</v>
       </c>
-      <c r="M20" s="8">
+      <c r="M20" s="10">
         <v>11</v>
       </c>
-      <c r="N20" s="8">
+      <c r="N20" s="10">
         <v>12</v>
       </c>
-      <c r="O20" s="8">
+      <c r="O20" s="10">
         <v>13</v>
       </c>
-      <c r="P20" s="8">
+      <c r="P20" s="10">
         <v>14</v>
       </c>
-      <c r="Q20" s="8">
+      <c r="Q20" s="10">
         <v>15</v>
       </c>
-      <c r="R20" s="8">
+      <c r="R20" s="10">
         <v>16</v>
       </c>
-      <c r="S20" s="13">
+      <c r="S20" s="11">
         <v>17</v>
       </c>
-      <c r="T20" s="10"/>
+      <c r="T20" s="8"/>
     </row>
     <row r="21" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
-      <c r="E21" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="F21" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="30"/>
-      <c r="H21" s="30"/>
-      <c r="I21" s="30"/>
-      <c r="J21" s="30"/>
-      <c r="K21" s="30"/>
-      <c r="L21" s="3" t="s">
+      <c r="A21" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
+      <c r="S21" s="35"/>
+    </row>
+    <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B22" s="22" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="23"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="22" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="23"/>
+      <c r="G22" s="23"/>
+      <c r="H22" s="23"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="K22" s="23"/>
+      <c r="L22" s="23"/>
+      <c r="M22" s="23"/>
+      <c r="N22" s="24"/>
+      <c r="O22" s="22" t="s">
+        <v>56</v>
+      </c>
+      <c r="P22" s="23"/>
+      <c r="Q22" s="23"/>
+      <c r="R22" s="23"/>
+      <c r="S22" s="24"/>
+    </row>
+    <row r="23" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="M21" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="N21" s="30"/>
-      <c r="O21" s="30"/>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="30"/>
-      <c r="S21" s="3" t="s">
+      <c r="B23" s="33" t="s">
+        <v>206</v>
+      </c>
+      <c r="C23" s="34"/>
+      <c r="D23" s="34"/>
+      <c r="E23" s="34"/>
+      <c r="F23" s="34"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="34"/>
+      <c r="I23" s="34"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
+      <c r="S23" s="35"/>
+    </row>
+    <row r="26" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="43" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="43" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>59</v>
-      </c>
-      <c r="C22" s="27"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="28"/>
-      <c r="J22" s="26" t="s">
-        <v>61</v>
-      </c>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="28"/>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>197</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="B27" s="47" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="C27" s="46"/>
+      <c r="D27" s="46"/>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="48"/>
+      <c r="I27" s="45" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="J27" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="K27" s="25"/>
+      <c r="L27" s="25"/>
+      <c r="M27" s="25"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="25"/>
+      <c r="P27" s="25"/>
+      <c r="Q27" s="26"/>
+    </row>
+    <row r="28" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="43" t="s">
         <v>202</v>
       </c>
+      <c r="B28" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="49" t="s">
+        <v>207</v>
+      </c>
+      <c r="K28" s="49"/>
+      <c r="L28" s="49"/>
+      <c r="M28" s="49"/>
+      <c r="N28" s="49"/>
+      <c r="O28" s="49"/>
+      <c r="P28" s="49"/>
+      <c r="Q28" s="51"/>
+    </row>
+    <row r="29" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="43" t="s">
+        <v>204</v>
+      </c>
+      <c r="B29" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="52" t="s">
+        <v>208</v>
+      </c>
+      <c r="K29" s="52"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="52"/>
+      <c r="N29" s="52"/>
+      <c r="O29" s="52"/>
+      <c r="P29" s="52"/>
+      <c r="Q29" s="53"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="20">
+    <mergeCell ref="B28:I28"/>
+    <mergeCell ref="B29:I29"/>
+    <mergeCell ref="B23:S23"/>
+    <mergeCell ref="B21:S21"/>
+    <mergeCell ref="F11:L11"/>
+    <mergeCell ref="J27:Q27"/>
+    <mergeCell ref="J28:Q28"/>
+    <mergeCell ref="J29:Q29"/>
     <mergeCell ref="C11:E11"/>
+    <mergeCell ref="J10:L10"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="B27:H27"/>
     <mergeCell ref="K9:L9"/>
     <mergeCell ref="E22:I22"/>
     <mergeCell ref="J22:N22"/>
     <mergeCell ref="O22:S22"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="F21:K21"/>
-    <mergeCell ref="M21:R21"/>
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="F9:J9"/>
     <mergeCell ref="C9:E9"/>
@@ -2128,35 +2287,35 @@
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>73</v>
-      </c>
-      <c r="D1" s="19" t="s">
+    <row r="1" spans="1:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" s="19" t="s">
+      <c r="E1" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" s="19" t="s">
-        <v>64</v>
+      <c r="G1" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="H1" s="16" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2165,10 +2324,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F2">
         <v>10</v>
@@ -2182,7 +2341,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2191,10 +2350,10 @@
         <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F3">
         <v>10</v>
@@ -2208,7 +2367,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2217,10 +2376,10 @@
         <v>3</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="E4" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F4">
         <v>10</v>
@@ -2234,7 +2393,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2243,10 +2402,10 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="E5" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F5">
         <v>100</v>
@@ -2260,7 +2419,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2269,10 +2428,10 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="E6" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F6">
         <v>1000</v>
@@ -2286,7 +2445,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -2295,10 +2454,10 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E7" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F7">
         <v>1000</v>
@@ -2312,7 +2471,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2321,10 +2480,10 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="E8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F8">
         <v>100</v>
@@ -2336,12 +2495,12 @@
         <v>14</v>
       </c>
       <c r="K8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -2350,10 +2509,10 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="E9" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F9">
         <v>100</v>
@@ -2365,12 +2524,12 @@
         <v>14</v>
       </c>
       <c r="K9" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2379,10 +2538,10 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="E10" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F10">
         <v>100</v>
@@ -2396,7 +2555,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -2405,10 +2564,10 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F11">
         <v>100</v>
@@ -2422,7 +2581,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2431,10 +2590,10 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E12" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="F12">
         <v>100</v>
@@ -2448,7 +2607,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2457,10 +2616,10 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F13">
         <v>10</v>
@@ -2474,7 +2633,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -2483,10 +2642,10 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="F14">
         <v>10</v>
@@ -2500,7 +2659,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -2509,10 +2668,10 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="E15" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F15">
         <v>100</v>
@@ -2526,7 +2685,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -2535,10 +2694,10 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="E16" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F16">
         <v>100</v>
@@ -2552,7 +2711,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -2561,10 +2720,10 @@
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="E17" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F17">
         <v>100</v>
@@ -2578,7 +2737,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -2587,10 +2746,10 @@
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="E18" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F18">
         <v>100</v>
@@ -2604,7 +2763,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -2613,10 +2772,10 @@
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F19">
         <v>100</v>
@@ -2683,26 +2842,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>72</v>
+      <c r="A1" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D1" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="E1" s="23"/>
+        <v>70</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" s="19"/>
       <c r="F1" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B2">
         <v>24</v>
@@ -2710,13 +2869,13 @@
       <c r="C2">
         <v>10</v>
       </c>
-      <c r="D2" s="20" t="s">
-        <v>109</v>
+      <c r="D2" s="17" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B3">
         <v>24</v>
@@ -2724,13 +2883,13 @@
       <c r="C3">
         <v>11</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>108</v>
+      <c r="D3" s="17" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>16</v>
@@ -2738,13 +2897,13 @@
       <c r="C4">
         <v>13</v>
       </c>
-      <c r="D4" s="20" t="s">
-        <v>106</v>
+      <c r="D4" s="17" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>16</v>
@@ -2752,13 +2911,13 @@
       <c r="C5">
         <v>13</v>
       </c>
-      <c r="D5" s="20" t="s">
-        <v>106</v>
+      <c r="D5" s="17" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B6">
         <v>16</v>
@@ -2766,16 +2925,16 @@
       <c r="C6">
         <v>12</v>
       </c>
-      <c r="D6" s="20" t="s">
-        <v>107</v>
+      <c r="D6" s="17" t="s">
+        <v>101</v>
       </c>
       <c r="F6" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B7">
         <v>13</v>
@@ -2783,16 +2942,16 @@
       <c r="C7">
         <v>10</v>
       </c>
-      <c r="D7" s="20" t="s">
-        <v>104</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>105</v>
+      <c r="D7" s="17" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="17" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="F14" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -2830,16 +2989,16 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2847,13 +3006,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D2" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2861,16 +3020,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C3" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="J3" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2878,16 +3037,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D4" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2895,16 +3054,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="C5" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2912,16 +3071,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="J6" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2929,13 +3088,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2943,13 +3102,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C8" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D8" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2957,13 +3116,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2971,13 +3130,13 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D10" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2985,13 +3144,13 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C11" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D11" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2999,13 +3158,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D12" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -3013,13 +3172,13 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C13" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -3027,13 +3186,13 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C14" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D14" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -3041,13 +3200,13 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C15" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D15" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -3055,13 +3214,13 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D16" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -3069,13 +3228,13 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C17" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D17" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -3168,13 +3327,13 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C35" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="D35" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -3350,20 +3509,20 @@
     <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>78</v>
-      </c>
-      <c r="B1" s="18" t="s">
+    <row r="1" spans="1:3" s="15" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="15" t="s">
         <v>77</v>
-      </c>
-      <c r="C1" s="18" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3374,7 +3533,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -3385,7 +3544,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="B4">
         <v>2</v>
@@ -3396,7 +3555,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -3566,7 +3725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44D6762A-FC32-4463-BC95-D819309C4519}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
@@ -3580,30 +3739,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C1" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D1" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="E1" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="35" t="s">
-        <v>174</v>
+      <c r="C2" s="31" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3611,10 +3770,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3622,10 +3781,10 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D4" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3633,10 +3792,10 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="D5" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3644,10 +3803,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="D6" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3655,10 +3814,10 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="D7" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3666,10 +3825,10 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="D8" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3677,10 +3836,10 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D9" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3688,10 +3847,10 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D10" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3699,10 +3858,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D11" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3710,10 +3869,10 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3721,10 +3880,10 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="D13" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3732,10 +3891,10 @@
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="D14" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3743,10 +3902,10 @@
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3754,10 +3913,10 @@
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="D16" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
@@ -3765,10 +3924,10 @@
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="D17" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
@@ -3776,10 +3935,10 @@
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D18" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
@@ -3787,10 +3946,10 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D19" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
@@ -3798,10 +3957,10 @@
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="D20" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
@@ -3809,10 +3968,10 @@
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D21" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
@@ -3820,10 +3979,10 @@
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="D22" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
@@ -3831,10 +3990,10 @@
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D23" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
@@ -3842,10 +4001,10 @@
         <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D24" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
@@ -3853,10 +4012,10 @@
         <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D25" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
@@ -3864,10 +4023,10 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D26" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
@@ -3875,10 +4034,10 @@
         <v>26</v>
       </c>
       <c r="C27" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D27" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
@@ -3886,10 +4045,10 @@
         <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D28" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
@@ -3897,10 +4056,10 @@
         <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D29" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
@@ -3908,10 +4067,10 @@
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D30" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
@@ -3956,7 +4115,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="B40">
         <v>1</v>
@@ -4051,8 +4210,8 @@
       <c r="B58">
         <v>19</v>
       </c>
-      <c r="C58" s="35" t="s">
-        <v>174</v>
+      <c r="C58" s="31" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">

</xml_diff>